<commit_message>
update profile url handling and cf fields
</commit_message>
<xml_diff>
--- a/ProfileCF/input.xlsx
+++ b/ProfileCF/input.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11207"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/aaron.cummins/Documents/migration/ProfileCF/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/aaron.cummins/Documents/migration/ProfileUrls/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DEBEEFAD-630B-054C-B86B-4526EE4DF84E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD17294D-7D28-8A47-8A32-FDEA75F13D01}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1420" yWindow="760" windowWidth="28820" windowHeight="18880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4742" uniqueCount="4741">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5225" uniqueCount="5224">
   <si>
     <t>URL</t>
   </si>
@@ -14247,6 +14247,1455 @@
   </si>
   <si>
     <t>zwilliam</t>
+  </si>
+  <si>
+    <t>abarron</t>
+  </si>
+  <si>
+    <t>acheh</t>
+  </si>
+  <si>
+    <t>akraut</t>
+  </si>
+  <si>
+    <t>alevent</t>
+  </si>
+  <si>
+    <t>angelad</t>
+  </si>
+  <si>
+    <t>anmandel</t>
+  </si>
+  <si>
+    <t>aoliver</t>
+  </si>
+  <si>
+    <t>aperry</t>
+  </si>
+  <si>
+    <t>aserra</t>
+  </si>
+  <si>
+    <t>awu</t>
+  </si>
+  <si>
+    <t>azelle</t>
+  </si>
+  <si>
+    <t>bbird</t>
+  </si>
+  <si>
+    <t>bdicker</t>
+  </si>
+  <si>
+    <t>bdiggs</t>
+  </si>
+  <si>
+    <t>beisner</t>
+  </si>
+  <si>
+    <t>bennett</t>
+  </si>
+  <si>
+    <t>berendz</t>
+  </si>
+  <si>
+    <t>bernhofe</t>
+  </si>
+  <si>
+    <t>bforst</t>
+  </si>
+  <si>
+    <t>bfst</t>
+  </si>
+  <si>
+    <t>bkaufman</t>
+  </si>
+  <si>
+    <t>blecker</t>
+  </si>
+  <si>
+    <t>bmccar</t>
+  </si>
+  <si>
+    <t>bromzek</t>
+  </si>
+  <si>
+    <t>bschill</t>
+  </si>
+  <si>
+    <t>bsiman</t>
+  </si>
+  <si>
+    <t>bwillia</t>
+  </si>
+  <si>
+    <t>byates</t>
+  </si>
+  <si>
+    <t>carberry</t>
+  </si>
+  <si>
+    <t>cdegreg</t>
+  </si>
+  <si>
+    <t>chardwi</t>
+  </si>
+  <si>
+    <t>chdez</t>
+  </si>
+  <si>
+    <t>cho</t>
+  </si>
+  <si>
+    <t>cjennin</t>
+  </si>
+  <si>
+    <t>clewis</t>
+  </si>
+  <si>
+    <t>clusane</t>
+  </si>
+  <si>
+    <t>colleen</t>
+  </si>
+  <si>
+    <t>corr</t>
+  </si>
+  <si>
+    <t>cschnei</t>
+  </si>
+  <si>
+    <t>cweissb</t>
+  </si>
+  <si>
+    <t>daarons</t>
+  </si>
+  <si>
+    <t>davenpor</t>
+  </si>
+  <si>
+    <t>dbrenner</t>
+  </si>
+  <si>
+    <t>dclarke</t>
+  </si>
+  <si>
+    <t>dcpayne</t>
+  </si>
+  <si>
+    <t>dcrosby</t>
+  </si>
+  <si>
+    <t>dfong</t>
+  </si>
+  <si>
+    <t>dgolash</t>
+  </si>
+  <si>
+    <t>dkahn</t>
+  </si>
+  <si>
+    <t>dkhamba</t>
+  </si>
+  <si>
+    <t>dkoenig</t>
+  </si>
+  <si>
+    <t>dmartin</t>
+  </si>
+  <si>
+    <t>dr-y</t>
+  </si>
+  <si>
+    <t>drodier</t>
+  </si>
+  <si>
+    <t>dsadker</t>
+  </si>
+  <si>
+    <t>dsinger</t>
+  </si>
+  <si>
+    <t>durant</t>
+  </si>
+  <si>
+    <t>dvogel</t>
+  </si>
+  <si>
+    <t>dzauder</t>
+  </si>
+  <si>
+    <t>eblaes</t>
+  </si>
+  <si>
+    <t>echow</t>
+  </si>
+  <si>
+    <t>efeder</t>
+  </si>
+  <si>
+    <t>elang</t>
+  </si>
+  <si>
+    <t>elliott</t>
+  </si>
+  <si>
+    <t>elliottm</t>
+  </si>
+  <si>
+    <t>elving</t>
+  </si>
+  <si>
+    <t>emer_abarron</t>
+  </si>
+  <si>
+    <t>emer_abravan</t>
+  </si>
+  <si>
+    <t>emer_acheh</t>
+  </si>
+  <si>
+    <t>emer_aclarke</t>
+  </si>
+  <si>
+    <t>emer_alevent</t>
+  </si>
+  <si>
+    <t>emer_amirkin</t>
+  </si>
+  <si>
+    <t>emer_anmandel</t>
+  </si>
+  <si>
+    <t>emer_aphelps</t>
+  </si>
+  <si>
+    <t>emer_areimann</t>
+  </si>
+  <si>
+    <t>emer_aserra</t>
+  </si>
+  <si>
+    <t>emer_awu</t>
+  </si>
+  <si>
+    <t>emer_azelle</t>
+  </si>
+  <si>
+    <t>emer_bbird</t>
+  </si>
+  <si>
+    <t>emer_bburke</t>
+  </si>
+  <si>
+    <t>emer_bdicker</t>
+  </si>
+  <si>
+    <t>emer_bdiggs</t>
+  </si>
+  <si>
+    <t>emer_bforst</t>
+  </si>
+  <si>
+    <t>emer_bfst</t>
+  </si>
+  <si>
+    <t>emer_bkaufman</t>
+  </si>
+  <si>
+    <t>emer_bradlow</t>
+  </si>
+  <si>
+    <t>emer_bromzek</t>
+  </si>
+  <si>
+    <t>emer_bschill</t>
+  </si>
+  <si>
+    <t>emer_bsiman</t>
+  </si>
+  <si>
+    <t>emer_bwillia</t>
+  </si>
+  <si>
+    <t>emer_carberry</t>
+  </si>
+  <si>
+    <t>emer_cdegreg</t>
+  </si>
+  <si>
+    <t>emer_chdez</t>
+  </si>
+  <si>
+    <t>emer_cjennin</t>
+  </si>
+  <si>
+    <t>emer_clewis</t>
+  </si>
+  <si>
+    <t>emer_clusane</t>
+  </si>
+  <si>
+    <t>emer_cochran</t>
+  </si>
+  <si>
+    <t>emer_cweissb</t>
+  </si>
+  <si>
+    <t>emer_daarons</t>
+  </si>
+  <si>
+    <t>emer_daaronson</t>
+  </si>
+  <si>
+    <t>emer_davenpor</t>
+  </si>
+  <si>
+    <t>emer_dbreyere</t>
+  </si>
+  <si>
+    <t>emer_dburkart</t>
+  </si>
+  <si>
+    <t>emer_dchavkin</t>
+  </si>
+  <si>
+    <t>emer_dcrosby</t>
+  </si>
+  <si>
+    <t>emer_ddurand</t>
+  </si>
+  <si>
+    <t>emer_dgolash</t>
+  </si>
+  <si>
+    <t>emer_dkahn</t>
+  </si>
+  <si>
+    <t>emer_dkhamba</t>
+  </si>
+  <si>
+    <t>emer_dkoenig</t>
+  </si>
+  <si>
+    <t>emer_doolittle</t>
+  </si>
+  <si>
+    <t>emer_dr-y</t>
+  </si>
+  <si>
+    <t>emer_drodier</t>
+  </si>
+  <si>
+    <t>emer_dsaari</t>
+  </si>
+  <si>
+    <t>emer_dsadker</t>
+  </si>
+  <si>
+    <t>emer_dsinger</t>
+  </si>
+  <si>
+    <t>emer_durant</t>
+  </si>
+  <si>
+    <t>emer_echow</t>
+  </si>
+  <si>
+    <t>emer_ehan</t>
+  </si>
+  <si>
+    <t>emer_ehanus</t>
+  </si>
+  <si>
+    <t>emer_ehirano</t>
+  </si>
+  <si>
+    <t>emer_ekovacic-fleischer</t>
+  </si>
+  <si>
+    <t>emer_elliott</t>
+  </si>
+  <si>
+    <t>emer_emachlin</t>
+  </si>
+  <si>
+    <t>emer_enayat</t>
+  </si>
+  <si>
+    <t>emer_eschuetze</t>
+  </si>
+  <si>
+    <t>emer_estes</t>
+  </si>
+  <si>
+    <t>emer_ezich</t>
+  </si>
+  <si>
+    <t>emer_fcarson</t>
+  </si>
+  <si>
+    <t>emer_fcheru</t>
+  </si>
+  <si>
+    <t>emer_fredj</t>
+  </si>
+  <si>
+    <t>emer_gadams</t>
+  </si>
+  <si>
+    <t>emer_gburkhar</t>
+  </si>
+  <si>
+    <t>emer_gharnde</t>
+  </si>
+  <si>
+    <t>emer_ghumphr</t>
+  </si>
+  <si>
+    <t>emer_gmessersmith</t>
+  </si>
+  <si>
+    <t>emer_gray</t>
+  </si>
+  <si>
+    <t>emer_haig</t>
+  </si>
+  <si>
+    <t>emer_headlee</t>
+  </si>
+  <si>
+    <t>emer_hjohnson</t>
+  </si>
+  <si>
+    <t>emer_hkusterer</t>
+  </si>
+  <si>
+    <t>emer_hlanga</t>
+  </si>
+  <si>
+    <t>emer_holzsagr</t>
+  </si>
+  <si>
+    <t>emer_hschwar</t>
+  </si>
+  <si>
+    <t>emer_htaylor</t>
+  </si>
+  <si>
+    <t>emer_ibroder</t>
+  </si>
+  <si>
+    <t>emer_ikarazikas</t>
+  </si>
+  <si>
+    <t>emer_ilchang</t>
+  </si>
+  <si>
+    <t>emer_jbaker</t>
+  </si>
+  <si>
+    <t>emer_jdougla</t>
+  </si>
+  <si>
+    <t>emer_jfishel</t>
+  </si>
+  <si>
+    <t>emer_jflug</t>
+  </si>
+  <si>
+    <t>emer_jgirard</t>
+  </si>
+  <si>
+    <t>emer_jgray</t>
+  </si>
+  <si>
+    <t>emer_jheintz</t>
+  </si>
+  <si>
+    <t>emer_jklein</t>
+  </si>
+  <si>
+    <t>emer_jloesbe</t>
+  </si>
+  <si>
+    <t>emer_jmalloy</t>
+  </si>
+  <si>
+    <t>emer_jradner</t>
+  </si>
+  <si>
+    <t>emer_jreiman</t>
+  </si>
+  <si>
+    <t>emer_jrich</t>
+  </si>
+  <si>
+    <t>emer_jsapiey</t>
+  </si>
+  <si>
+    <t>emer_jschill</t>
+  </si>
+  <si>
+    <t>emer_jsieg</t>
+  </si>
+  <si>
+    <t>emer_jswasy</t>
+  </si>
+  <si>
+    <t>emer_jwhite</t>
+  </si>
+  <si>
+    <t>emer_jwisman</t>
+  </si>
+  <si>
+    <t>emer_kalman</t>
+  </si>
+  <si>
+    <t>emer_kcm</t>
+  </si>
+  <si>
+    <t>emer_kebaker</t>
+  </si>
+  <si>
+    <t>emer_kkravet</t>
+  </si>
+  <si>
+    <t>emer_kmoyer</t>
+  </si>
+  <si>
+    <t>emer_kovacic</t>
+  </si>
+  <si>
+    <t>emer_langbei</t>
+  </si>
+  <si>
+    <t>emer_lasalle</t>
+  </si>
+  <si>
+    <t>emer_lbradlow</t>
+  </si>
+  <si>
+    <t>emer_lburke</t>
+  </si>
+  <si>
+    <t>emer_lcrone</t>
+  </si>
+  <si>
+    <t>emer_lewis</t>
+  </si>
+  <si>
+    <t>emer_linowes</t>
+  </si>
+  <si>
+    <t>emer_lkorin</t>
+  </si>
+  <si>
+    <t>emer_lnyce</t>
+  </si>
+  <si>
+    <t>emer_lsawers</t>
+  </si>
+  <si>
+    <t>emer_lubrano</t>
+  </si>
+  <si>
+    <t>emer_lwolfso</t>
+  </si>
+  <si>
+    <t>emer_lynn.fox</t>
+  </si>
+  <si>
+    <t>emer_marshak</t>
+  </si>
+  <si>
+    <t>emer_mccurdy</t>
+  </si>
+  <si>
+    <t>emer_mehlert</t>
+  </si>
+  <si>
+    <t>emer_mgarrar</t>
+  </si>
+  <si>
+    <t>emer_mgraham</t>
+  </si>
+  <si>
+    <t>emer_mhammer</t>
+  </si>
+  <si>
+    <t>emer_mmead</t>
+  </si>
+  <si>
+    <t>emer_mowlana</t>
+  </si>
+  <si>
+    <t>emer_moxman</t>
+  </si>
+  <si>
+    <t>emer_msampson</t>
+  </si>
+  <si>
+    <t>emer_mshapir</t>
+  </si>
+  <si>
+    <t>emer_msiegel</t>
+  </si>
+  <si>
+    <t>emer_msklarew</t>
+  </si>
+  <si>
+    <t>emer_mstahr</t>
+  </si>
+  <si>
+    <t>emer_mussell</t>
+  </si>
+  <si>
+    <t>emer_nabramo</t>
+  </si>
+  <si>
+    <t>emer_nabravanel</t>
+  </si>
+  <si>
+    <t>emer_nbaker</t>
+  </si>
+  <si>
+    <t>emer_nbaron</t>
+  </si>
+  <si>
+    <t>emer_nbennett</t>
+  </si>
+  <si>
+    <t>emer_nblaes</t>
+  </si>
+  <si>
+    <t>emer_nbroude</t>
+  </si>
+  <si>
+    <t>emer_nclarke</t>
+  </si>
+  <si>
+    <t>emer_nharris</t>
+  </si>
+  <si>
+    <t>emer_nkokus</t>
+  </si>
+  <si>
+    <t>emer_nlewis</t>
+  </si>
+  <si>
+    <t>emer_npoliko</t>
+  </si>
+  <si>
+    <t>emer_nraskin</t>
+  </si>
+  <si>
+    <t>emer_nrobertson</t>
+  </si>
+  <si>
+    <t>emer_nscott</t>
+  </si>
+  <si>
+    <t>emer_okaufman</t>
+  </si>
+  <si>
+    <t>emer_openay</t>
+  </si>
+  <si>
+    <t>emer_oreynolds</t>
+  </si>
+  <si>
+    <t>emer_orojer</t>
+  </si>
+  <si>
+    <t>emer_pascale</t>
+  </si>
+  <si>
+    <t>emer_pbrenne</t>
+  </si>
+  <si>
+    <t>emer_pcthanh</t>
+  </si>
+  <si>
+    <t>emer_persaud</t>
+  </si>
+  <si>
+    <t>emer_pheng-b</t>
+  </si>
+  <si>
+    <t>emer_pike</t>
+  </si>
+  <si>
+    <t>emer_pjacoby</t>
+  </si>
+  <si>
+    <t>emer_pkehoe</t>
+  </si>
+  <si>
+    <t>emer_pkumar</t>
+  </si>
+  <si>
+    <t>emer_pospiesz</t>
+  </si>
+  <si>
+    <t>emer_potomac</t>
+  </si>
+  <si>
+    <t>emer_prevots</t>
+  </si>
+  <si>
+    <t>emer_pscrib</t>
+  </si>
+  <si>
+    <t>emer_pwapner</t>
+  </si>
+  <si>
+    <t>emer_raskin</t>
+  </si>
+  <si>
+    <t>emer_rbloom</t>
+  </si>
+  <si>
+    <t>emer_rbowles</t>
+  </si>
+  <si>
+    <t>emer_rbreit</t>
+  </si>
+  <si>
+    <t>emer_rchinloy</t>
+  </si>
+  <si>
+    <t>emer_reiss</t>
+  </si>
+  <si>
+    <t>emer_rfisher</t>
+  </si>
+  <si>
+    <t>emer_rhahnel</t>
+  </si>
+  <si>
+    <t>emer_richard</t>
+  </si>
+  <si>
+    <t>emer_riddick</t>
+  </si>
+  <si>
+    <t>emer_rlerman</t>
+  </si>
+  <si>
+    <t>emer_rlosey</t>
+  </si>
+  <si>
+    <t>emer_rodamar</t>
+  </si>
+  <si>
+    <t>emer_rsemiat</t>
+  </si>
+  <si>
+    <t>emer_rstack</t>
+  </si>
+  <si>
+    <t>emer_rstone</t>
+  </si>
+  <si>
+    <t>emer_rstreit</t>
+  </si>
+  <si>
+    <t>emer_rubenst</t>
+  </si>
+  <si>
+    <t>emer_rweiner</t>
+  </si>
+  <si>
+    <t>emer_sbennett</t>
+  </si>
+  <si>
+    <t>emer_scohen</t>
+  </si>
+  <si>
+    <t>emer_sdernburg</t>
+  </si>
+  <si>
+    <t>emer_sdibacco</t>
+  </si>
+  <si>
+    <t>emer_segnan</t>
+  </si>
+  <si>
+    <t>emer_seldin</t>
+  </si>
+  <si>
+    <t>emer_sholmbe</t>
+  </si>
+  <si>
+    <t>emer_simpson</t>
+  </si>
+  <si>
+    <t>emer_slewis</t>
+  </si>
+  <si>
+    <t>emer_slong</t>
+  </si>
+  <si>
+    <t>emer_slotnic</t>
+  </si>
+  <si>
+    <t>emer_smardin</t>
+  </si>
+  <si>
+    <t>emer_smarien</t>
+  </si>
+  <si>
+    <t>emer_smirkin</t>
+  </si>
+  <si>
+    <t>emer_sneilsn</t>
+  </si>
+  <si>
+    <t>emer_sparker</t>
+  </si>
+  <si>
+    <t>emer_svidy</t>
+  </si>
+  <si>
+    <t>emer_swallow</t>
+  </si>
+  <si>
+    <t>emer_tbergin</t>
+  </si>
+  <si>
+    <t>emer_tmcginnies</t>
+  </si>
+  <si>
+    <t>emer_tmilstein</t>
+  </si>
+  <si>
+    <t>emer_tphelps</t>
+  </si>
+  <si>
+    <t>emer_tspringer</t>
+  </si>
+  <si>
+    <t>emer_tthompson</t>
+  </si>
+  <si>
+    <t>emer_tvaughn</t>
+  </si>
+  <si>
+    <t>emer_vandyke</t>
+  </si>
+  <si>
+    <t>emer_vaughn</t>
+  </si>
+  <si>
+    <t>emer_volkema</t>
+  </si>
+  <si>
+    <t>emer_vrenios</t>
+  </si>
+  <si>
+    <t>emer_vselman</t>
+  </si>
+  <si>
+    <t>emer_vstalli</t>
+  </si>
+  <si>
+    <t>emer_wachtel</t>
+  </si>
+  <si>
+    <t>emer_wcbanta</t>
+  </si>
+  <si>
+    <t>emer_wdelone</t>
+  </si>
+  <si>
+    <t>emer_wigfallw</t>
+  </si>
+  <si>
+    <t>emer_wlm</t>
+  </si>
+  <si>
+    <t>emer_wpike</t>
+  </si>
+  <si>
+    <t>emer_ybulmash</t>
+  </si>
+  <si>
+    <t>emer_ycoward</t>
+  </si>
+  <si>
+    <t>emer_yhendrix</t>
+  </si>
+  <si>
+    <t>emer_ymccann</t>
+  </si>
+  <si>
+    <t>emer_ymccarthy</t>
+  </si>
+  <si>
+    <t>emer_ypolikoff</t>
+  </si>
+  <si>
+    <t>emer_ysiegel</t>
+  </si>
+  <si>
+    <t>emer_zapatka</t>
+  </si>
+  <si>
+    <t>enayat</t>
+  </si>
+  <si>
+    <t>enibley</t>
+  </si>
+  <si>
+    <t>estes</t>
+  </si>
+  <si>
+    <t>fcarson</t>
+  </si>
+  <si>
+    <t>fcheru</t>
+  </si>
+  <si>
+    <t>fdubois</t>
+  </si>
+  <si>
+    <t>frank</t>
+  </si>
+  <si>
+    <t>fredj</t>
+  </si>
+  <si>
+    <t>fturaj</t>
+  </si>
+  <si>
+    <t>gadams</t>
+  </si>
+  <si>
+    <t>garnold</t>
+  </si>
+  <si>
+    <t>gburkhar</t>
+  </si>
+  <si>
+    <t>gharnde</t>
+  </si>
+  <si>
+    <t>ghumphr</t>
+  </si>
+  <si>
+    <t>gmccann</t>
+  </si>
+  <si>
+    <t>gmoomau</t>
+  </si>
+  <si>
+    <t>gmuel</t>
+  </si>
+  <si>
+    <t>grandas</t>
+  </si>
+  <si>
+    <t>gray</t>
+  </si>
+  <si>
+    <t>gtford</t>
+  </si>
+  <si>
+    <t>guttman</t>
+  </si>
+  <si>
+    <t>gyoung</t>
+  </si>
+  <si>
+    <t>haig</t>
+  </si>
+  <si>
+    <t>headlee</t>
+  </si>
+  <si>
+    <t>hershber</t>
+  </si>
+  <si>
+    <t>holzsagr</t>
+  </si>
+  <si>
+    <t>hschwar</t>
+  </si>
+  <si>
+    <t>htaylor</t>
+  </si>
+  <si>
+    <t>hunterd</t>
+  </si>
+  <si>
+    <t>ibroder</t>
+  </si>
+  <si>
+    <t>ilchang</t>
+  </si>
+  <si>
+    <t>jfishel</t>
+  </si>
+  <si>
+    <t>jflug</t>
+  </si>
+  <si>
+    <t>jgardner</t>
+  </si>
+  <si>
+    <t>jgray</t>
+  </si>
+  <si>
+    <t>jheintz</t>
+  </si>
+  <si>
+    <t>jklein</t>
+  </si>
+  <si>
+    <t>jloesbe</t>
+  </si>
+  <si>
+    <t>jmalloy</t>
+  </si>
+  <si>
+    <t>jorgens</t>
+  </si>
+  <si>
+    <t>jradner</t>
+  </si>
+  <si>
+    <t>jreiman</t>
+  </si>
+  <si>
+    <t>jrich</t>
+  </si>
+  <si>
+    <t>jsapiey</t>
+  </si>
+  <si>
+    <t>jschill</t>
+  </si>
+  <si>
+    <t>jsieg</t>
+  </si>
+  <si>
+    <t>jsulliva</t>
+  </si>
+  <si>
+    <t>jswasy</t>
+  </si>
+  <si>
+    <t>jwhite</t>
+  </si>
+  <si>
+    <t>jwisman</t>
+  </si>
+  <si>
+    <t>jzich</t>
+  </si>
+  <si>
+    <t>kalman</t>
+  </si>
+  <si>
+    <t>kb5515a</t>
+  </si>
+  <si>
+    <t>kcm</t>
+  </si>
+  <si>
+    <t>kebaker</t>
+  </si>
+  <si>
+    <t>kincade</t>
+  </si>
+  <si>
+    <t>kittrie</t>
+  </si>
+  <si>
+    <t>kkravet</t>
+  </si>
+  <si>
+    <t>kmoyer</t>
+  </si>
+  <si>
+    <t>koehler</t>
+  </si>
+  <si>
+    <t>kovacic</t>
+  </si>
+  <si>
+    <t>lajohns</t>
+  </si>
+  <si>
+    <t>langbei</t>
+  </si>
+  <si>
+    <t>lasalle</t>
+  </si>
+  <si>
+    <t>lchase</t>
+  </si>
+  <si>
+    <t>lcrone</t>
+  </si>
+  <si>
+    <t>lf2149a</t>
+  </si>
+  <si>
+    <t>lieber</t>
+  </si>
+  <si>
+    <t>linowes</t>
+  </si>
+  <si>
+    <t>lnyce</t>
+  </si>
+  <si>
+    <t>lubrano</t>
+  </si>
+  <si>
+    <t>lwolfso</t>
+  </si>
+  <si>
+    <t>lwoott</t>
+  </si>
+  <si>
+    <t>marshak</t>
+  </si>
+  <si>
+    <t>mccurdy</t>
+  </si>
+  <si>
+    <t>mehlert</t>
+  </si>
+  <si>
+    <t>mgarrar</t>
+  </si>
+  <si>
+    <t>mgraham</t>
+  </si>
+  <si>
+    <t>mgreenb</t>
+  </si>
+  <si>
+    <t>mhammer</t>
+  </si>
+  <si>
+    <t>mhastak</t>
+  </si>
+  <si>
+    <t>mmazis</t>
+  </si>
+  <si>
+    <t>mmead</t>
+  </si>
+  <si>
+    <t>mmintz</t>
+  </si>
+  <si>
+    <t>mowlana</t>
+  </si>
+  <si>
+    <t>moxman</t>
+  </si>
+  <si>
+    <t>mrocz</t>
+  </si>
+  <si>
+    <t>msampson</t>
+  </si>
+  <si>
+    <t>mshapir</t>
+  </si>
+  <si>
+    <t>msiegel</t>
+  </si>
+  <si>
+    <t>msklarew</t>
+  </si>
+  <si>
+    <t>mstruel</t>
+  </si>
+  <si>
+    <t>mussell</t>
+  </si>
+  <si>
+    <t>nbaron</t>
+  </si>
+  <si>
+    <t>nbroude</t>
+  </si>
+  <si>
+    <t>nharris</t>
+  </si>
+  <si>
+    <t>npoliko</t>
+  </si>
+  <si>
+    <t>orentlic</t>
+  </si>
+  <si>
+    <t>orojer</t>
+  </si>
+  <si>
+    <t>pascale</t>
+  </si>
+  <si>
+    <t>pbrenne</t>
+  </si>
+  <si>
+    <t>pcthanh</t>
+  </si>
+  <si>
+    <t>pearson</t>
+  </si>
+  <si>
+    <t>persaud</t>
+  </si>
+  <si>
+    <t>peynir</t>
+  </si>
+  <si>
+    <t>pheng-b</t>
+  </si>
+  <si>
+    <t>pike</t>
+  </si>
+  <si>
+    <t>pjacoby</t>
+  </si>
+  <si>
+    <t>pkehoe</t>
+  </si>
+  <si>
+    <t>pospiesz</t>
+  </si>
+  <si>
+    <t>potomac</t>
+  </si>
+  <si>
+    <t>prevots</t>
+  </si>
+  <si>
+    <t>pscrib</t>
+  </si>
+  <si>
+    <t>pstarr</t>
+  </si>
+  <si>
+    <t>psykes</t>
+  </si>
+  <si>
+    <t>pwapner</t>
+  </si>
+  <si>
+    <t>pwaters</t>
+  </si>
+  <si>
+    <t>quainton</t>
+  </si>
+  <si>
+    <t>ranieri</t>
+  </si>
+  <si>
+    <t>rblair</t>
+  </si>
+  <si>
+    <t>rbloom</t>
+  </si>
+  <si>
+    <t>rbreit</t>
+  </si>
+  <si>
+    <t>rcleary</t>
+  </si>
+  <si>
+    <t>rdiners</t>
+  </si>
+  <si>
+    <t>reiss</t>
+  </si>
+  <si>
+    <t>rfisher</t>
+  </si>
+  <si>
+    <t>rfox</t>
+  </si>
+  <si>
+    <t>rgregg</t>
+  </si>
+  <si>
+    <t>rhahnel</t>
+  </si>
+  <si>
+    <t>richard</t>
+  </si>
+  <si>
+    <t>rkarch</t>
+  </si>
+  <si>
+    <t>rlane</t>
+  </si>
+  <si>
+    <t>rlerman</t>
+  </si>
+  <si>
+    <t>rlosey</t>
+  </si>
+  <si>
+    <t>rmccann</t>
+  </si>
+  <si>
+    <t>robertjohnson</t>
+  </si>
+  <si>
+    <t>Rsemiat</t>
+  </si>
+  <si>
+    <t>rsmolka</t>
+  </si>
+  <si>
+    <t>rstack</t>
+  </si>
+  <si>
+    <t>rstone</t>
+  </si>
+  <si>
+    <t>rstreit</t>
+  </si>
+  <si>
+    <t>rtobias</t>
+  </si>
+  <si>
+    <t>rubenst</t>
+  </si>
+  <si>
+    <t>rweiner</t>
+  </si>
+  <si>
+    <t>sarnold</t>
+  </si>
+  <si>
+    <t>schot</t>
+  </si>
+  <si>
+    <t>scohen</t>
+  </si>
+  <si>
+    <t>segnan</t>
+  </si>
+  <si>
+    <t>seldin</t>
+  </si>
+  <si>
+    <t>sfowler</t>
+  </si>
+  <si>
+    <t>sgrant</t>
+  </si>
+  <si>
+    <t>shallec</t>
+  </si>
+  <si>
+    <t>shammo</t>
+  </si>
+  <si>
+    <t>shelfor</t>
+  </si>
+  <si>
+    <t>sholmbe</t>
+  </si>
+  <si>
+    <t>skramer</t>
+  </si>
+  <si>
+    <t>slaughlin</t>
+  </si>
+  <si>
+    <t>slewis</t>
+  </si>
+  <si>
+    <t>slotnic</t>
+  </si>
+  <si>
+    <t>smardin</t>
+  </si>
+  <si>
+    <t>smarien</t>
+  </si>
+  <si>
+    <t>sneilsn</t>
+  </si>
+  <si>
+    <t>sparker</t>
+  </si>
+  <si>
+    <t>striner</t>
+  </si>
+  <si>
+    <t>swallow</t>
+  </si>
+  <si>
+    <t>tbergin</t>
+  </si>
+  <si>
+    <t>terryd</t>
+  </si>
+  <si>
+    <t>tesconi</t>
+  </si>
+  <si>
+    <t>tmrocz2002@yahoo.com</t>
+  </si>
+  <si>
+    <t>tomasko</t>
+  </si>
+  <si>
+    <t>tphelps</t>
+  </si>
+  <si>
+    <t>vandyke</t>
+  </si>
+  <si>
+    <t>vfrench</t>
+  </si>
+  <si>
+    <t>vidalort</t>
+  </si>
+  <si>
+    <t>volkema</t>
+  </si>
+  <si>
+    <t>vrenios</t>
+  </si>
+  <si>
+    <t>vselman</t>
+  </si>
+  <si>
+    <t>vstalli</t>
+  </si>
+  <si>
+    <t>wachtel</t>
+  </si>
+  <si>
+    <t>waterhouse</t>
+  </si>
+  <si>
+    <t>wcbanta</t>
+  </si>
+  <si>
+    <t>wdelone</t>
+  </si>
+  <si>
+    <t>wjc</t>
+  </si>
+  <si>
+    <t>wlm</t>
+  </si>
+  <si>
+    <t>zapatka</t>
   </si>
 </sst>
 </file>
@@ -14595,10 +16044,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:B4733"/>
+  <dimension ref="A1:B5216"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection activeCell="A2" sqref="A2:A5216"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -41765,6 +43214,2421 @@
     <row r="4733" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A4733" s="1" t="s">
         <v>4740</v>
+      </c>
+    </row>
+    <row r="4734" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A4734" s="1" t="s">
+        <v>4741</v>
+      </c>
+    </row>
+    <row r="4735" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A4735" s="1" t="s">
+        <v>4742</v>
+      </c>
+    </row>
+    <row r="4736" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A4736" s="1" t="s">
+        <v>4743</v>
+      </c>
+    </row>
+    <row r="4737" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A4737" s="1" t="s">
+        <v>4744</v>
+      </c>
+    </row>
+    <row r="4738" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A4738" s="1" t="s">
+        <v>4745</v>
+      </c>
+    </row>
+    <row r="4739" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A4739" s="1" t="s">
+        <v>4746</v>
+      </c>
+    </row>
+    <row r="4740" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A4740" s="1" t="s">
+        <v>4747</v>
+      </c>
+    </row>
+    <row r="4741" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A4741" s="1" t="s">
+        <v>4748</v>
+      </c>
+    </row>
+    <row r="4742" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A4742" s="1" t="s">
+        <v>4749</v>
+      </c>
+    </row>
+    <row r="4743" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A4743" s="1" t="s">
+        <v>4750</v>
+      </c>
+    </row>
+    <row r="4744" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A4744" s="1" t="s">
+        <v>4751</v>
+      </c>
+    </row>
+    <row r="4745" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A4745" s="1" t="s">
+        <v>4752</v>
+      </c>
+    </row>
+    <row r="4746" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A4746" s="1" t="s">
+        <v>4753</v>
+      </c>
+    </row>
+    <row r="4747" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A4747" s="1" t="s">
+        <v>4754</v>
+      </c>
+    </row>
+    <row r="4748" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A4748" s="1" t="s">
+        <v>4755</v>
+      </c>
+    </row>
+    <row r="4749" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A4749" s="1" t="s">
+        <v>4756</v>
+      </c>
+    </row>
+    <row r="4750" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A4750" s="1" t="s">
+        <v>4757</v>
+      </c>
+    </row>
+    <row r="4751" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A4751" s="1" t="s">
+        <v>4758</v>
+      </c>
+    </row>
+    <row r="4752" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A4752" s="1" t="s">
+        <v>4759</v>
+      </c>
+    </row>
+    <row r="4753" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A4753" s="1" t="s">
+        <v>4760</v>
+      </c>
+    </row>
+    <row r="4754" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A4754" s="1" t="s">
+        <v>4761</v>
+      </c>
+    </row>
+    <row r="4755" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A4755" s="1" t="s">
+        <v>4762</v>
+      </c>
+    </row>
+    <row r="4756" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A4756" s="1" t="s">
+        <v>4763</v>
+      </c>
+    </row>
+    <row r="4757" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A4757" s="1" t="s">
+        <v>4764</v>
+      </c>
+    </row>
+    <row r="4758" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A4758" s="1" t="s">
+        <v>4765</v>
+      </c>
+    </row>
+    <row r="4759" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A4759" s="1" t="s">
+        <v>4766</v>
+      </c>
+    </row>
+    <row r="4760" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A4760" s="1" t="s">
+        <v>4767</v>
+      </c>
+    </row>
+    <row r="4761" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A4761" s="1" t="s">
+        <v>4768</v>
+      </c>
+    </row>
+    <row r="4762" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A4762" s="1" t="s">
+        <v>4769</v>
+      </c>
+    </row>
+    <row r="4763" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A4763" s="1" t="s">
+        <v>4770</v>
+      </c>
+    </row>
+    <row r="4764" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A4764" s="1" t="s">
+        <v>4771</v>
+      </c>
+    </row>
+    <row r="4765" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A4765" s="1" t="s">
+        <v>4772</v>
+      </c>
+    </row>
+    <row r="4766" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A4766" s="1" t="s">
+        <v>4773</v>
+      </c>
+    </row>
+    <row r="4767" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A4767" s="1" t="s">
+        <v>4774</v>
+      </c>
+    </row>
+    <row r="4768" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A4768" s="1" t="s">
+        <v>4775</v>
+      </c>
+    </row>
+    <row r="4769" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A4769" s="1" t="s">
+        <v>4776</v>
+      </c>
+    </row>
+    <row r="4770" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A4770" s="1" t="s">
+        <v>4777</v>
+      </c>
+    </row>
+    <row r="4771" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A4771" s="1" t="s">
+        <v>4778</v>
+      </c>
+    </row>
+    <row r="4772" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A4772" s="1" t="s">
+        <v>4779</v>
+      </c>
+    </row>
+    <row r="4773" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A4773" s="1" t="s">
+        <v>4780</v>
+      </c>
+    </row>
+    <row r="4774" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A4774" s="1" t="s">
+        <v>4781</v>
+      </c>
+    </row>
+    <row r="4775" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A4775" s="1" t="s">
+        <v>4782</v>
+      </c>
+    </row>
+    <row r="4776" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A4776" s="1" t="s">
+        <v>4783</v>
+      </c>
+    </row>
+    <row r="4777" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A4777" s="1" t="s">
+        <v>4784</v>
+      </c>
+    </row>
+    <row r="4778" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A4778" s="1" t="s">
+        <v>4785</v>
+      </c>
+    </row>
+    <row r="4779" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A4779" s="1" t="s">
+        <v>4786</v>
+      </c>
+    </row>
+    <row r="4780" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A4780" s="1" t="s">
+        <v>4787</v>
+      </c>
+    </row>
+    <row r="4781" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A4781" s="1" t="s">
+        <v>4788</v>
+      </c>
+    </row>
+    <row r="4782" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A4782" s="1" t="s">
+        <v>4789</v>
+      </c>
+    </row>
+    <row r="4783" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A4783" s="1" t="s">
+        <v>4790</v>
+      </c>
+    </row>
+    <row r="4784" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A4784" s="1" t="s">
+        <v>4791</v>
+      </c>
+    </row>
+    <row r="4785" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A4785" s="1" t="s">
+        <v>4792</v>
+      </c>
+    </row>
+    <row r="4786" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A4786" s="1" t="s">
+        <v>4793</v>
+      </c>
+    </row>
+    <row r="4787" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A4787" s="1" t="s">
+        <v>4794</v>
+      </c>
+    </row>
+    <row r="4788" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A4788" s="1" t="s">
+        <v>4795</v>
+      </c>
+    </row>
+    <row r="4789" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A4789" s="1" t="s">
+        <v>4796</v>
+      </c>
+    </row>
+    <row r="4790" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A4790" s="1" t="s">
+        <v>4797</v>
+      </c>
+    </row>
+    <row r="4791" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A4791" s="1" t="s">
+        <v>4798</v>
+      </c>
+    </row>
+    <row r="4792" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A4792" s="1" t="s">
+        <v>4799</v>
+      </c>
+    </row>
+    <row r="4793" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A4793" s="1" t="s">
+        <v>4800</v>
+      </c>
+    </row>
+    <row r="4794" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A4794" s="1" t="s">
+        <v>4801</v>
+      </c>
+    </row>
+    <row r="4795" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A4795" s="1" t="s">
+        <v>4802</v>
+      </c>
+    </row>
+    <row r="4796" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A4796" s="1" t="s">
+        <v>4803</v>
+      </c>
+    </row>
+    <row r="4797" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A4797" s="1" t="s">
+        <v>4804</v>
+      </c>
+    </row>
+    <row r="4798" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A4798" s="1" t="s">
+        <v>4805</v>
+      </c>
+    </row>
+    <row r="4799" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A4799" s="1" t="s">
+        <v>4806</v>
+      </c>
+    </row>
+    <row r="4800" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A4800" s="1" t="s">
+        <v>4807</v>
+      </c>
+    </row>
+    <row r="4801" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A4801" s="1" t="s">
+        <v>4808</v>
+      </c>
+    </row>
+    <row r="4802" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A4802" s="1" t="s">
+        <v>4809</v>
+      </c>
+    </row>
+    <row r="4803" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A4803" s="1" t="s">
+        <v>4810</v>
+      </c>
+    </row>
+    <row r="4804" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A4804" s="1" t="s">
+        <v>4811</v>
+      </c>
+    </row>
+    <row r="4805" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A4805" s="1" t="s">
+        <v>4812</v>
+      </c>
+    </row>
+    <row r="4806" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A4806" s="1" t="s">
+        <v>4813</v>
+      </c>
+    </row>
+    <row r="4807" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A4807" s="1" t="s">
+        <v>4814</v>
+      </c>
+    </row>
+    <row r="4808" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A4808" s="1" t="s">
+        <v>4815</v>
+      </c>
+    </row>
+    <row r="4809" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A4809" s="1" t="s">
+        <v>4816</v>
+      </c>
+    </row>
+    <row r="4810" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A4810" s="1" t="s">
+        <v>4817</v>
+      </c>
+    </row>
+    <row r="4811" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A4811" s="1" t="s">
+        <v>4818</v>
+      </c>
+    </row>
+    <row r="4812" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A4812" s="1" t="s">
+        <v>4819</v>
+      </c>
+    </row>
+    <row r="4813" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A4813" s="1" t="s">
+        <v>4820</v>
+      </c>
+    </row>
+    <row r="4814" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A4814" s="1" t="s">
+        <v>4821</v>
+      </c>
+    </row>
+    <row r="4815" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A4815" s="1" t="s">
+        <v>4822</v>
+      </c>
+    </row>
+    <row r="4816" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A4816" s="1" t="s">
+        <v>4823</v>
+      </c>
+    </row>
+    <row r="4817" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A4817" s="1" t="s">
+        <v>4824</v>
+      </c>
+    </row>
+    <row r="4818" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A4818" s="1" t="s">
+        <v>4825</v>
+      </c>
+    </row>
+    <row r="4819" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A4819" s="1" t="s">
+        <v>4826</v>
+      </c>
+    </row>
+    <row r="4820" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A4820" s="1" t="s">
+        <v>4827</v>
+      </c>
+    </row>
+    <row r="4821" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A4821" s="1" t="s">
+        <v>4828</v>
+      </c>
+    </row>
+    <row r="4822" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A4822" s="1" t="s">
+        <v>4829</v>
+      </c>
+    </row>
+    <row r="4823" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A4823" s="1" t="s">
+        <v>4830</v>
+      </c>
+    </row>
+    <row r="4824" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A4824" s="1" t="s">
+        <v>4831</v>
+      </c>
+    </row>
+    <row r="4825" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A4825" s="1" t="s">
+        <v>4832</v>
+      </c>
+    </row>
+    <row r="4826" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A4826" s="1" t="s">
+        <v>4833</v>
+      </c>
+    </row>
+    <row r="4827" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A4827" s="1" t="s">
+        <v>4834</v>
+      </c>
+    </row>
+    <row r="4828" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A4828" s="1" t="s">
+        <v>4835</v>
+      </c>
+    </row>
+    <row r="4829" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A4829" s="1" t="s">
+        <v>4836</v>
+      </c>
+    </row>
+    <row r="4830" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A4830" s="1" t="s">
+        <v>4837</v>
+      </c>
+    </row>
+    <row r="4831" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A4831" s="1" t="s">
+        <v>4838</v>
+      </c>
+    </row>
+    <row r="4832" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A4832" s="1" t="s">
+        <v>4839</v>
+      </c>
+    </row>
+    <row r="4833" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A4833" s="1" t="s">
+        <v>4840</v>
+      </c>
+    </row>
+    <row r="4834" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A4834" s="1" t="s">
+        <v>4841</v>
+      </c>
+    </row>
+    <row r="4835" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A4835" s="1" t="s">
+        <v>4842</v>
+      </c>
+    </row>
+    <row r="4836" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A4836" s="1" t="s">
+        <v>4843</v>
+      </c>
+    </row>
+    <row r="4837" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A4837" s="1" t="s">
+        <v>4844</v>
+      </c>
+    </row>
+    <row r="4838" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A4838" s="1" t="s">
+        <v>4845</v>
+      </c>
+    </row>
+    <row r="4839" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A4839" s="1" t="s">
+        <v>4846</v>
+      </c>
+    </row>
+    <row r="4840" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A4840" s="1" t="s">
+        <v>4847</v>
+      </c>
+    </row>
+    <row r="4841" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A4841" s="1" t="s">
+        <v>4848</v>
+      </c>
+    </row>
+    <row r="4842" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A4842" s="1" t="s">
+        <v>4849</v>
+      </c>
+    </row>
+    <row r="4843" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A4843" s="1" t="s">
+        <v>4850</v>
+      </c>
+    </row>
+    <row r="4844" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A4844" s="1" t="s">
+        <v>4851</v>
+      </c>
+    </row>
+    <row r="4845" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A4845" s="1" t="s">
+        <v>4852</v>
+      </c>
+    </row>
+    <row r="4846" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A4846" s="1" t="s">
+        <v>4853</v>
+      </c>
+    </row>
+    <row r="4847" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A4847" s="1" t="s">
+        <v>4854</v>
+      </c>
+    </row>
+    <row r="4848" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A4848" s="1" t="s">
+        <v>4855</v>
+      </c>
+    </row>
+    <row r="4849" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A4849" s="1" t="s">
+        <v>4856</v>
+      </c>
+    </row>
+    <row r="4850" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A4850" s="1" t="s">
+        <v>4857</v>
+      </c>
+    </row>
+    <row r="4851" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A4851" s="1" t="s">
+        <v>4858</v>
+      </c>
+    </row>
+    <row r="4852" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A4852" s="1" t="s">
+        <v>4859</v>
+      </c>
+    </row>
+    <row r="4853" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A4853" s="1" t="s">
+        <v>4860</v>
+      </c>
+    </row>
+    <row r="4854" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A4854" s="1" t="s">
+        <v>4861</v>
+      </c>
+    </row>
+    <row r="4855" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A4855" s="1" t="s">
+        <v>4862</v>
+      </c>
+    </row>
+    <row r="4856" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A4856" s="1" t="s">
+        <v>4863</v>
+      </c>
+    </row>
+    <row r="4857" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A4857" s="1" t="s">
+        <v>4864</v>
+      </c>
+    </row>
+    <row r="4858" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A4858" s="1" t="s">
+        <v>4865</v>
+      </c>
+    </row>
+    <row r="4859" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A4859" s="1" t="s">
+        <v>4866</v>
+      </c>
+    </row>
+    <row r="4860" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A4860" s="1" t="s">
+        <v>4867</v>
+      </c>
+    </row>
+    <row r="4861" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A4861" s="1" t="s">
+        <v>4868</v>
+      </c>
+    </row>
+    <row r="4862" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A4862" s="1" t="s">
+        <v>4869</v>
+      </c>
+    </row>
+    <row r="4863" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A4863" s="1" t="s">
+        <v>4870</v>
+      </c>
+    </row>
+    <row r="4864" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A4864" s="1" t="s">
+        <v>4871</v>
+      </c>
+    </row>
+    <row r="4865" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A4865" s="1" t="s">
+        <v>4872</v>
+      </c>
+    </row>
+    <row r="4866" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A4866" s="1" t="s">
+        <v>4873</v>
+      </c>
+    </row>
+    <row r="4867" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A4867" s="1" t="s">
+        <v>4874</v>
+      </c>
+    </row>
+    <row r="4868" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A4868" s="1" t="s">
+        <v>4875</v>
+      </c>
+    </row>
+    <row r="4869" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A4869" s="1" t="s">
+        <v>4876</v>
+      </c>
+    </row>
+    <row r="4870" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A4870" s="1" t="s">
+        <v>4877</v>
+      </c>
+    </row>
+    <row r="4871" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A4871" s="1" t="s">
+        <v>4878</v>
+      </c>
+    </row>
+    <row r="4872" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A4872" s="1" t="s">
+        <v>4879</v>
+      </c>
+    </row>
+    <row r="4873" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A4873" s="1" t="s">
+        <v>4880</v>
+      </c>
+    </row>
+    <row r="4874" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A4874" s="1" t="s">
+        <v>4881</v>
+      </c>
+    </row>
+    <row r="4875" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A4875" s="1" t="s">
+        <v>4882</v>
+      </c>
+    </row>
+    <row r="4876" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A4876" s="1" t="s">
+        <v>4883</v>
+      </c>
+    </row>
+    <row r="4877" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A4877" s="1" t="s">
+        <v>4884</v>
+      </c>
+    </row>
+    <row r="4878" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A4878" s="1" t="s">
+        <v>4885</v>
+      </c>
+    </row>
+    <row r="4879" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A4879" s="1" t="s">
+        <v>4886</v>
+      </c>
+    </row>
+    <row r="4880" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A4880" s="1" t="s">
+        <v>4887</v>
+      </c>
+    </row>
+    <row r="4881" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A4881" s="1" t="s">
+        <v>4888</v>
+      </c>
+    </row>
+    <row r="4882" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A4882" s="1" t="s">
+        <v>4889</v>
+      </c>
+    </row>
+    <row r="4883" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A4883" s="1" t="s">
+        <v>4890</v>
+      </c>
+    </row>
+    <row r="4884" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A4884" s="1" t="s">
+        <v>4891</v>
+      </c>
+    </row>
+    <row r="4885" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A4885" s="1" t="s">
+        <v>4892</v>
+      </c>
+    </row>
+    <row r="4886" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A4886" s="1" t="s">
+        <v>4893</v>
+      </c>
+    </row>
+    <row r="4887" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A4887" s="1" t="s">
+        <v>4894</v>
+      </c>
+    </row>
+    <row r="4888" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A4888" s="1" t="s">
+        <v>4895</v>
+      </c>
+    </row>
+    <row r="4889" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A4889" s="1" t="s">
+        <v>4896</v>
+      </c>
+    </row>
+    <row r="4890" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A4890" s="1" t="s">
+        <v>4897</v>
+      </c>
+    </row>
+    <row r="4891" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A4891" s="1" t="s">
+        <v>4898</v>
+      </c>
+    </row>
+    <row r="4892" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A4892" s="1" t="s">
+        <v>4899</v>
+      </c>
+    </row>
+    <row r="4893" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A4893" s="1" t="s">
+        <v>4900</v>
+      </c>
+    </row>
+    <row r="4894" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A4894" s="1" t="s">
+        <v>4901</v>
+      </c>
+    </row>
+    <row r="4895" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A4895" s="1" t="s">
+        <v>4902</v>
+      </c>
+    </row>
+    <row r="4896" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A4896" s="1" t="s">
+        <v>4903</v>
+      </c>
+    </row>
+    <row r="4897" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A4897" s="1" t="s">
+        <v>4904</v>
+      </c>
+    </row>
+    <row r="4898" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A4898" s="1" t="s">
+        <v>4905</v>
+      </c>
+    </row>
+    <row r="4899" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A4899" s="1" t="s">
+        <v>4906</v>
+      </c>
+    </row>
+    <row r="4900" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A4900" s="1" t="s">
+        <v>4907</v>
+      </c>
+    </row>
+    <row r="4901" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A4901" s="1" t="s">
+        <v>4908</v>
+      </c>
+    </row>
+    <row r="4902" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A4902" s="1" t="s">
+        <v>4909</v>
+      </c>
+    </row>
+    <row r="4903" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A4903" s="1" t="s">
+        <v>4910</v>
+      </c>
+    </row>
+    <row r="4904" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A4904" s="1" t="s">
+        <v>4911</v>
+      </c>
+    </row>
+    <row r="4905" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A4905" s="1" t="s">
+        <v>4912</v>
+      </c>
+    </row>
+    <row r="4906" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A4906" s="1" t="s">
+        <v>4913</v>
+      </c>
+    </row>
+    <row r="4907" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A4907" s="1" t="s">
+        <v>4914</v>
+      </c>
+    </row>
+    <row r="4908" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A4908" s="1" t="s">
+        <v>4915</v>
+      </c>
+    </row>
+    <row r="4909" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A4909" s="1" t="s">
+        <v>4916</v>
+      </c>
+    </row>
+    <row r="4910" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A4910" s="1" t="s">
+        <v>4917</v>
+      </c>
+    </row>
+    <row r="4911" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A4911" s="1" t="s">
+        <v>4918</v>
+      </c>
+    </row>
+    <row r="4912" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A4912" s="1" t="s">
+        <v>4919</v>
+      </c>
+    </row>
+    <row r="4913" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A4913" s="1" t="s">
+        <v>4920</v>
+      </c>
+    </row>
+    <row r="4914" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A4914" s="1" t="s">
+        <v>4921</v>
+      </c>
+    </row>
+    <row r="4915" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A4915" s="1" t="s">
+        <v>4922</v>
+      </c>
+    </row>
+    <row r="4916" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A4916" s="1" t="s">
+        <v>4923</v>
+      </c>
+    </row>
+    <row r="4917" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A4917" s="1" t="s">
+        <v>4924</v>
+      </c>
+    </row>
+    <row r="4918" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A4918" s="1" t="s">
+        <v>4925</v>
+      </c>
+    </row>
+    <row r="4919" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A4919" s="1" t="s">
+        <v>4926</v>
+      </c>
+    </row>
+    <row r="4920" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A4920" s="1" t="s">
+        <v>4927</v>
+      </c>
+    </row>
+    <row r="4921" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A4921" s="1" t="s">
+        <v>4928</v>
+      </c>
+    </row>
+    <row r="4922" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A4922" s="1" t="s">
+        <v>4929</v>
+      </c>
+    </row>
+    <row r="4923" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A4923" s="1" t="s">
+        <v>4930</v>
+      </c>
+    </row>
+    <row r="4924" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A4924" s="1" t="s">
+        <v>4931</v>
+      </c>
+    </row>
+    <row r="4925" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A4925" s="1" t="s">
+        <v>4932</v>
+      </c>
+    </row>
+    <row r="4926" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A4926" s="1" t="s">
+        <v>4933</v>
+      </c>
+    </row>
+    <row r="4927" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A4927" s="1" t="s">
+        <v>4934</v>
+      </c>
+    </row>
+    <row r="4928" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A4928" s="1" t="s">
+        <v>4935</v>
+      </c>
+    </row>
+    <row r="4929" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A4929" s="1" t="s">
+        <v>4936</v>
+      </c>
+    </row>
+    <row r="4930" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A4930" s="1" t="s">
+        <v>4937</v>
+      </c>
+    </row>
+    <row r="4931" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A4931" s="1" t="s">
+        <v>4938</v>
+      </c>
+    </row>
+    <row r="4932" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A4932" s="1" t="s">
+        <v>4939</v>
+      </c>
+    </row>
+    <row r="4933" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A4933" s="1" t="s">
+        <v>4940</v>
+      </c>
+    </row>
+    <row r="4934" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A4934" s="1" t="s">
+        <v>4941</v>
+      </c>
+    </row>
+    <row r="4935" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A4935" s="1" t="s">
+        <v>4942</v>
+      </c>
+    </row>
+    <row r="4936" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A4936" s="1" t="s">
+        <v>4943</v>
+      </c>
+    </row>
+    <row r="4937" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A4937" s="1" t="s">
+        <v>4944</v>
+      </c>
+    </row>
+    <row r="4938" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A4938" s="1" t="s">
+        <v>4945</v>
+      </c>
+    </row>
+    <row r="4939" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A4939" s="1" t="s">
+        <v>4946</v>
+      </c>
+    </row>
+    <row r="4940" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A4940" s="1" t="s">
+        <v>4947</v>
+      </c>
+    </row>
+    <row r="4941" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A4941" s="1" t="s">
+        <v>4948</v>
+      </c>
+    </row>
+    <row r="4942" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A4942" s="1" t="s">
+        <v>4949</v>
+      </c>
+    </row>
+    <row r="4943" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A4943" s="1" t="s">
+        <v>4950</v>
+      </c>
+    </row>
+    <row r="4944" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A4944" s="1" t="s">
+        <v>4951</v>
+      </c>
+    </row>
+    <row r="4945" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A4945" s="1" t="s">
+        <v>4952</v>
+      </c>
+    </row>
+    <row r="4946" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A4946" s="1" t="s">
+        <v>4953</v>
+      </c>
+    </row>
+    <row r="4947" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A4947" s="1" t="s">
+        <v>4954</v>
+      </c>
+    </row>
+    <row r="4948" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A4948" s="1" t="s">
+        <v>4955</v>
+      </c>
+    </row>
+    <row r="4949" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A4949" s="1" t="s">
+        <v>4956</v>
+      </c>
+    </row>
+    <row r="4950" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A4950" s="1" t="s">
+        <v>4957</v>
+      </c>
+    </row>
+    <row r="4951" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A4951" s="1" t="s">
+        <v>4958</v>
+      </c>
+    </row>
+    <row r="4952" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A4952" s="1" t="s">
+        <v>4959</v>
+      </c>
+    </row>
+    <row r="4953" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A4953" s="1" t="s">
+        <v>4960</v>
+      </c>
+    </row>
+    <row r="4954" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A4954" s="1" t="s">
+        <v>4961</v>
+      </c>
+    </row>
+    <row r="4955" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A4955" s="1" t="s">
+        <v>4962</v>
+      </c>
+    </row>
+    <row r="4956" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A4956" s="1" t="s">
+        <v>4963</v>
+      </c>
+    </row>
+    <row r="4957" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A4957" s="1" t="s">
+        <v>4964</v>
+      </c>
+    </row>
+    <row r="4958" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A4958" s="1" t="s">
+        <v>4965</v>
+      </c>
+    </row>
+    <row r="4959" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A4959" s="1" t="s">
+        <v>4966</v>
+      </c>
+    </row>
+    <row r="4960" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A4960" s="1" t="s">
+        <v>4967</v>
+      </c>
+    </row>
+    <row r="4961" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A4961" s="1" t="s">
+        <v>4968</v>
+      </c>
+    </row>
+    <row r="4962" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A4962" s="1" t="s">
+        <v>4969</v>
+      </c>
+    </row>
+    <row r="4963" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A4963" s="1" t="s">
+        <v>4970</v>
+      </c>
+    </row>
+    <row r="4964" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A4964" s="1" t="s">
+        <v>4971</v>
+      </c>
+    </row>
+    <row r="4965" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A4965" s="1" t="s">
+        <v>4972</v>
+      </c>
+    </row>
+    <row r="4966" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A4966" s="1" t="s">
+        <v>4973</v>
+      </c>
+    </row>
+    <row r="4967" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A4967" s="1" t="s">
+        <v>4974</v>
+      </c>
+    </row>
+    <row r="4968" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A4968" s="1" t="s">
+        <v>4975</v>
+      </c>
+    </row>
+    <row r="4969" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A4969" s="1" t="s">
+        <v>4976</v>
+      </c>
+    </row>
+    <row r="4970" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A4970" s="1" t="s">
+        <v>4977</v>
+      </c>
+    </row>
+    <row r="4971" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A4971" s="1" t="s">
+        <v>4978</v>
+      </c>
+    </row>
+    <row r="4972" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A4972" s="1" t="s">
+        <v>4979</v>
+      </c>
+    </row>
+    <row r="4973" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A4973" s="1" t="s">
+        <v>4980</v>
+      </c>
+    </row>
+    <row r="4974" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A4974" s="1" t="s">
+        <v>4981</v>
+      </c>
+    </row>
+    <row r="4975" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A4975" s="1" t="s">
+        <v>4982</v>
+      </c>
+    </row>
+    <row r="4976" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A4976" s="1" t="s">
+        <v>4983</v>
+      </c>
+    </row>
+    <row r="4977" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A4977" s="1" t="s">
+        <v>4984</v>
+      </c>
+    </row>
+    <row r="4978" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A4978" s="1" t="s">
+        <v>4985</v>
+      </c>
+    </row>
+    <row r="4979" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A4979" s="1" t="s">
+        <v>4986</v>
+      </c>
+    </row>
+    <row r="4980" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A4980" s="1" t="s">
+        <v>4987</v>
+      </c>
+    </row>
+    <row r="4981" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A4981" s="1" t="s">
+        <v>4988</v>
+      </c>
+    </row>
+    <row r="4982" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A4982" s="1" t="s">
+        <v>4989</v>
+      </c>
+    </row>
+    <row r="4983" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A4983" s="1" t="s">
+        <v>4990</v>
+      </c>
+    </row>
+    <row r="4984" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A4984" s="1" t="s">
+        <v>4991</v>
+      </c>
+    </row>
+    <row r="4985" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A4985" s="1" t="s">
+        <v>4992</v>
+      </c>
+    </row>
+    <row r="4986" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A4986" s="1" t="s">
+        <v>4993</v>
+      </c>
+    </row>
+    <row r="4987" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A4987" s="1" t="s">
+        <v>4994</v>
+      </c>
+    </row>
+    <row r="4988" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A4988" s="1" t="s">
+        <v>4995</v>
+      </c>
+    </row>
+    <row r="4989" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A4989" s="1" t="s">
+        <v>4996</v>
+      </c>
+    </row>
+    <row r="4990" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A4990" s="1" t="s">
+        <v>4997</v>
+      </c>
+    </row>
+    <row r="4991" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A4991" s="1" t="s">
+        <v>4998</v>
+      </c>
+    </row>
+    <row r="4992" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A4992" s="1" t="s">
+        <v>4999</v>
+      </c>
+    </row>
+    <row r="4993" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A4993" s="1" t="s">
+        <v>5000</v>
+      </c>
+    </row>
+    <row r="4994" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A4994" s="1" t="s">
+        <v>5001</v>
+      </c>
+    </row>
+    <row r="4995" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A4995" s="1" t="s">
+        <v>5002</v>
+      </c>
+    </row>
+    <row r="4996" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A4996" s="1" t="s">
+        <v>5003</v>
+      </c>
+    </row>
+    <row r="4997" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A4997" s="1" t="s">
+        <v>5004</v>
+      </c>
+    </row>
+    <row r="4998" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A4998" s="1" t="s">
+        <v>5005</v>
+      </c>
+    </row>
+    <row r="4999" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A4999" s="1" t="s">
+        <v>5006</v>
+      </c>
+    </row>
+    <row r="5000" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A5000" s="1" t="s">
+        <v>5007</v>
+      </c>
+    </row>
+    <row r="5001" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A5001" s="1" t="s">
+        <v>5008</v>
+      </c>
+    </row>
+    <row r="5002" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A5002" s="1" t="s">
+        <v>5009</v>
+      </c>
+    </row>
+    <row r="5003" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A5003" s="1" t="s">
+        <v>5010</v>
+      </c>
+    </row>
+    <row r="5004" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A5004" s="1" t="s">
+        <v>5011</v>
+      </c>
+    </row>
+    <row r="5005" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A5005" s="1" t="s">
+        <v>5012</v>
+      </c>
+    </row>
+    <row r="5006" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A5006" s="1" t="s">
+        <v>5013</v>
+      </c>
+    </row>
+    <row r="5007" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A5007" s="1" t="s">
+        <v>5014</v>
+      </c>
+    </row>
+    <row r="5008" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A5008" s="1" t="s">
+        <v>5015</v>
+      </c>
+    </row>
+    <row r="5009" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A5009" s="1" t="s">
+        <v>5016</v>
+      </c>
+    </row>
+    <row r="5010" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A5010" s="1" t="s">
+        <v>5017</v>
+      </c>
+    </row>
+    <row r="5011" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A5011" s="1" t="s">
+        <v>5018</v>
+      </c>
+    </row>
+    <row r="5012" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A5012" s="1" t="s">
+        <v>5019</v>
+      </c>
+    </row>
+    <row r="5013" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A5013" s="1" t="s">
+        <v>5020</v>
+      </c>
+    </row>
+    <row r="5014" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A5014" s="1" t="s">
+        <v>5021</v>
+      </c>
+    </row>
+    <row r="5015" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A5015" s="1" t="s">
+        <v>5022</v>
+      </c>
+    </row>
+    <row r="5016" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A5016" s="1" t="s">
+        <v>5023</v>
+      </c>
+    </row>
+    <row r="5017" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A5017" s="1" t="s">
+        <v>5024</v>
+      </c>
+    </row>
+    <row r="5018" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A5018" s="1" t="s">
+        <v>5025</v>
+      </c>
+    </row>
+    <row r="5019" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A5019" s="1" t="s">
+        <v>5026</v>
+      </c>
+    </row>
+    <row r="5020" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A5020" s="1" t="s">
+        <v>5027</v>
+      </c>
+    </row>
+    <row r="5021" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A5021" s="1" t="s">
+        <v>5028</v>
+      </c>
+    </row>
+    <row r="5022" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A5022" s="1" t="s">
+        <v>5029</v>
+      </c>
+    </row>
+    <row r="5023" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A5023" s="1" t="s">
+        <v>5030</v>
+      </c>
+    </row>
+    <row r="5024" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A5024" s="1" t="s">
+        <v>5031</v>
+      </c>
+    </row>
+    <row r="5025" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A5025" s="1" t="s">
+        <v>5032</v>
+      </c>
+    </row>
+    <row r="5026" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A5026" s="1" t="s">
+        <v>5033</v>
+      </c>
+    </row>
+    <row r="5027" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A5027" s="1" t="s">
+        <v>5034</v>
+      </c>
+    </row>
+    <row r="5028" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A5028" s="1" t="s">
+        <v>5035</v>
+      </c>
+    </row>
+    <row r="5029" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A5029" s="1" t="s">
+        <v>5036</v>
+      </c>
+    </row>
+    <row r="5030" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A5030" s="1" t="s">
+        <v>5037</v>
+      </c>
+    </row>
+    <row r="5031" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A5031" s="1" t="s">
+        <v>5038</v>
+      </c>
+    </row>
+    <row r="5032" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A5032" s="1" t="s">
+        <v>5039</v>
+      </c>
+    </row>
+    <row r="5033" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A5033" s="1" t="s">
+        <v>5040</v>
+      </c>
+    </row>
+    <row r="5034" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A5034" s="1" t="s">
+        <v>5041</v>
+      </c>
+    </row>
+    <row r="5035" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A5035" s="1" t="s">
+        <v>5042</v>
+      </c>
+    </row>
+    <row r="5036" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A5036" s="1" t="s">
+        <v>5043</v>
+      </c>
+    </row>
+    <row r="5037" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A5037" s="1" t="s">
+        <v>5044</v>
+      </c>
+    </row>
+    <row r="5038" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A5038" s="1" t="s">
+        <v>5045</v>
+      </c>
+    </row>
+    <row r="5039" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A5039" s="1" t="s">
+        <v>5046</v>
+      </c>
+    </row>
+    <row r="5040" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A5040" s="1" t="s">
+        <v>5047</v>
+      </c>
+    </row>
+    <row r="5041" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A5041" s="1" t="s">
+        <v>5048</v>
+      </c>
+    </row>
+    <row r="5042" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A5042" s="1" t="s">
+        <v>5049</v>
+      </c>
+    </row>
+    <row r="5043" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A5043" s="1" t="s">
+        <v>5050</v>
+      </c>
+    </row>
+    <row r="5044" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A5044" s="1" t="s">
+        <v>5051</v>
+      </c>
+    </row>
+    <row r="5045" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A5045" s="1" t="s">
+        <v>5052</v>
+      </c>
+    </row>
+    <row r="5046" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A5046" s="1" t="s">
+        <v>5053</v>
+      </c>
+    </row>
+    <row r="5047" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A5047" s="1" t="s">
+        <v>5054</v>
+      </c>
+    </row>
+    <row r="5048" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A5048" s="1" t="s">
+        <v>5055</v>
+      </c>
+    </row>
+    <row r="5049" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A5049" s="1" t="s">
+        <v>5056</v>
+      </c>
+    </row>
+    <row r="5050" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A5050" s="1" t="s">
+        <v>5057</v>
+      </c>
+    </row>
+    <row r="5051" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A5051" s="1" t="s">
+        <v>5058</v>
+      </c>
+    </row>
+    <row r="5052" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A5052" s="1" t="s">
+        <v>5059</v>
+      </c>
+    </row>
+    <row r="5053" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A5053" s="1" t="s">
+        <v>5060</v>
+      </c>
+    </row>
+    <row r="5054" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A5054" s="1" t="s">
+        <v>5061</v>
+      </c>
+    </row>
+    <row r="5055" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A5055" s="1" t="s">
+        <v>5062</v>
+      </c>
+    </row>
+    <row r="5056" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A5056" s="1" t="s">
+        <v>5063</v>
+      </c>
+    </row>
+    <row r="5057" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A5057" s="1" t="s">
+        <v>5064</v>
+      </c>
+    </row>
+    <row r="5058" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A5058" s="1" t="s">
+        <v>5065</v>
+      </c>
+    </row>
+    <row r="5059" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A5059" s="1" t="s">
+        <v>5066</v>
+      </c>
+    </row>
+    <row r="5060" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A5060" s="1" t="s">
+        <v>5067</v>
+      </c>
+    </row>
+    <row r="5061" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A5061" s="1" t="s">
+        <v>5068</v>
+      </c>
+    </row>
+    <row r="5062" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A5062" s="1" t="s">
+        <v>5069</v>
+      </c>
+    </row>
+    <row r="5063" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A5063" s="1" t="s">
+        <v>5070</v>
+      </c>
+    </row>
+    <row r="5064" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A5064" s="1" t="s">
+        <v>5071</v>
+      </c>
+    </row>
+    <row r="5065" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A5065" s="1" t="s">
+        <v>5072</v>
+      </c>
+    </row>
+    <row r="5066" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A5066" s="1" t="s">
+        <v>5073</v>
+      </c>
+    </row>
+    <row r="5067" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A5067" s="1" t="s">
+        <v>5074</v>
+      </c>
+    </row>
+    <row r="5068" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A5068" s="1" t="s">
+        <v>5075</v>
+      </c>
+    </row>
+    <row r="5069" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A5069" s="1" t="s">
+        <v>5076</v>
+      </c>
+    </row>
+    <row r="5070" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A5070" s="1" t="s">
+        <v>5077</v>
+      </c>
+    </row>
+    <row r="5071" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A5071" s="1" t="s">
+        <v>5078</v>
+      </c>
+    </row>
+    <row r="5072" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A5072" s="1" t="s">
+        <v>5079</v>
+      </c>
+    </row>
+    <row r="5073" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A5073" s="1" t="s">
+        <v>5080</v>
+      </c>
+    </row>
+    <row r="5074" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A5074" s="1" t="s">
+        <v>5081</v>
+      </c>
+    </row>
+    <row r="5075" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A5075" s="1" t="s">
+        <v>5082</v>
+      </c>
+    </row>
+    <row r="5076" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A5076" s="1" t="s">
+        <v>5083</v>
+      </c>
+    </row>
+    <row r="5077" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A5077" s="1" t="s">
+        <v>5084</v>
+      </c>
+    </row>
+    <row r="5078" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A5078" s="1" t="s">
+        <v>5085</v>
+      </c>
+    </row>
+    <row r="5079" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A5079" s="1" t="s">
+        <v>5086</v>
+      </c>
+    </row>
+    <row r="5080" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A5080" s="1" t="s">
+        <v>5087</v>
+      </c>
+    </row>
+    <row r="5081" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A5081" s="1" t="s">
+        <v>5088</v>
+      </c>
+    </row>
+    <row r="5082" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A5082" s="1" t="s">
+        <v>5089</v>
+      </c>
+    </row>
+    <row r="5083" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A5083" s="1" t="s">
+        <v>5090</v>
+      </c>
+    </row>
+    <row r="5084" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A5084" s="1" t="s">
+        <v>5091</v>
+      </c>
+    </row>
+    <row r="5085" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A5085" s="1" t="s">
+        <v>5092</v>
+      </c>
+    </row>
+    <row r="5086" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A5086" s="1" t="s">
+        <v>5093</v>
+      </c>
+    </row>
+    <row r="5087" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A5087" s="1" t="s">
+        <v>5094</v>
+      </c>
+    </row>
+    <row r="5088" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A5088" s="1" t="s">
+        <v>5095</v>
+      </c>
+    </row>
+    <row r="5089" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A5089" s="1" t="s">
+        <v>5096</v>
+      </c>
+    </row>
+    <row r="5090" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A5090" s="1" t="s">
+        <v>5097</v>
+      </c>
+    </row>
+    <row r="5091" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A5091" s="1" t="s">
+        <v>5098</v>
+      </c>
+    </row>
+    <row r="5092" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A5092" s="1" t="s">
+        <v>5099</v>
+      </c>
+    </row>
+    <row r="5093" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A5093" s="1" t="s">
+        <v>5100</v>
+      </c>
+    </row>
+    <row r="5094" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A5094" s="1" t="s">
+        <v>5101</v>
+      </c>
+    </row>
+    <row r="5095" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A5095" s="1" t="s">
+        <v>5102</v>
+      </c>
+    </row>
+    <row r="5096" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A5096" s="1" t="s">
+        <v>5103</v>
+      </c>
+    </row>
+    <row r="5097" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A5097" s="1" t="s">
+        <v>5104</v>
+      </c>
+    </row>
+    <row r="5098" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A5098" s="1" t="s">
+        <v>5105</v>
+      </c>
+    </row>
+    <row r="5099" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A5099" s="1" t="s">
+        <v>5106</v>
+      </c>
+    </row>
+    <row r="5100" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A5100" s="1" t="s">
+        <v>5107</v>
+      </c>
+    </row>
+    <row r="5101" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A5101" s="1" t="s">
+        <v>5108</v>
+      </c>
+    </row>
+    <row r="5102" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A5102" s="1" t="s">
+        <v>5109</v>
+      </c>
+    </row>
+    <row r="5103" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A5103" s="1" t="s">
+        <v>5110</v>
+      </c>
+    </row>
+    <row r="5104" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A5104" s="1" t="s">
+        <v>5111</v>
+      </c>
+    </row>
+    <row r="5105" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A5105" s="1" t="s">
+        <v>5112</v>
+      </c>
+    </row>
+    <row r="5106" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A5106" s="1" t="s">
+        <v>5113</v>
+      </c>
+    </row>
+    <row r="5107" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A5107" s="1" t="s">
+        <v>5114</v>
+      </c>
+    </row>
+    <row r="5108" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A5108" s="1" t="s">
+        <v>5115</v>
+      </c>
+    </row>
+    <row r="5109" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A5109" s="1" t="s">
+        <v>5116</v>
+      </c>
+    </row>
+    <row r="5110" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A5110" s="1" t="s">
+        <v>5117</v>
+      </c>
+    </row>
+    <row r="5111" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A5111" s="1" t="s">
+        <v>5118</v>
+      </c>
+    </row>
+    <row r="5112" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A5112" s="1" t="s">
+        <v>5119</v>
+      </c>
+    </row>
+    <row r="5113" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A5113" s="1" t="s">
+        <v>5120</v>
+      </c>
+    </row>
+    <row r="5114" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A5114" s="1" t="s">
+        <v>5121</v>
+      </c>
+    </row>
+    <row r="5115" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A5115" s="1" t="s">
+        <v>5122</v>
+      </c>
+    </row>
+    <row r="5116" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A5116" s="1" t="s">
+        <v>5123</v>
+      </c>
+    </row>
+    <row r="5117" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A5117" s="1" t="s">
+        <v>5124</v>
+      </c>
+    </row>
+    <row r="5118" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A5118" s="1" t="s">
+        <v>5125</v>
+      </c>
+    </row>
+    <row r="5119" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A5119" s="1" t="s">
+        <v>5126</v>
+      </c>
+    </row>
+    <row r="5120" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A5120" s="1" t="s">
+        <v>5127</v>
+      </c>
+    </row>
+    <row r="5121" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A5121" s="1" t="s">
+        <v>5128</v>
+      </c>
+    </row>
+    <row r="5122" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A5122" s="1" t="s">
+        <v>5129</v>
+      </c>
+    </row>
+    <row r="5123" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A5123" s="1" t="s">
+        <v>5130</v>
+      </c>
+    </row>
+    <row r="5124" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A5124" s="1" t="s">
+        <v>5131</v>
+      </c>
+    </row>
+    <row r="5125" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A5125" s="1" t="s">
+        <v>5132</v>
+      </c>
+    </row>
+    <row r="5126" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A5126" s="1" t="s">
+        <v>5133</v>
+      </c>
+    </row>
+    <row r="5127" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A5127" s="1" t="s">
+        <v>5134</v>
+      </c>
+    </row>
+    <row r="5128" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A5128" s="1" t="s">
+        <v>5135</v>
+      </c>
+    </row>
+    <row r="5129" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A5129" s="1" t="s">
+        <v>5136</v>
+      </c>
+    </row>
+    <row r="5130" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A5130" s="1" t="s">
+        <v>5137</v>
+      </c>
+    </row>
+    <row r="5131" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A5131" s="1" t="s">
+        <v>5138</v>
+      </c>
+    </row>
+    <row r="5132" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A5132" s="1" t="s">
+        <v>5139</v>
+      </c>
+    </row>
+    <row r="5133" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A5133" s="1" t="s">
+        <v>5140</v>
+      </c>
+    </row>
+    <row r="5134" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A5134" s="1" t="s">
+        <v>5141</v>
+      </c>
+    </row>
+    <row r="5135" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A5135" s="1" t="s">
+        <v>5142</v>
+      </c>
+    </row>
+    <row r="5136" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A5136" s="1" t="s">
+        <v>5143</v>
+      </c>
+    </row>
+    <row r="5137" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A5137" s="1" t="s">
+        <v>5144</v>
+      </c>
+    </row>
+    <row r="5138" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A5138" s="1" t="s">
+        <v>5145</v>
+      </c>
+    </row>
+    <row r="5139" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A5139" s="1" t="s">
+        <v>5146</v>
+      </c>
+    </row>
+    <row r="5140" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A5140" s="1" t="s">
+        <v>5147</v>
+      </c>
+    </row>
+    <row r="5141" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A5141" s="1" t="s">
+        <v>5148</v>
+      </c>
+    </row>
+    <row r="5142" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A5142" s="1" t="s">
+        <v>5149</v>
+      </c>
+    </row>
+    <row r="5143" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A5143" s="1" t="s">
+        <v>5150</v>
+      </c>
+    </row>
+    <row r="5144" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A5144" s="1" t="s">
+        <v>5151</v>
+      </c>
+    </row>
+    <row r="5145" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A5145" s="1" t="s">
+        <v>5152</v>
+      </c>
+    </row>
+    <row r="5146" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A5146" s="1" t="s">
+        <v>5153</v>
+      </c>
+    </row>
+    <row r="5147" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A5147" s="1" t="s">
+        <v>5154</v>
+      </c>
+    </row>
+    <row r="5148" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A5148" s="1" t="s">
+        <v>5155</v>
+      </c>
+    </row>
+    <row r="5149" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A5149" s="1" t="s">
+        <v>5156</v>
+      </c>
+    </row>
+    <row r="5150" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A5150" s="1" t="s">
+        <v>5157</v>
+      </c>
+    </row>
+    <row r="5151" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A5151" s="1" t="s">
+        <v>5158</v>
+      </c>
+    </row>
+    <row r="5152" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A5152" s="1" t="s">
+        <v>5159</v>
+      </c>
+    </row>
+    <row r="5153" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A5153" s="1" t="s">
+        <v>5160</v>
+      </c>
+    </row>
+    <row r="5154" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A5154" s="1" t="s">
+        <v>5161</v>
+      </c>
+    </row>
+    <row r="5155" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A5155" s="1" t="s">
+        <v>5162</v>
+      </c>
+    </row>
+    <row r="5156" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A5156" s="1" t="s">
+        <v>5163</v>
+      </c>
+    </row>
+    <row r="5157" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A5157" s="1" t="s">
+        <v>5164</v>
+      </c>
+    </row>
+    <row r="5158" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A5158" s="1" t="s">
+        <v>5165</v>
+      </c>
+    </row>
+    <row r="5159" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A5159" s="1" t="s">
+        <v>5166</v>
+      </c>
+    </row>
+    <row r="5160" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A5160" s="1" t="s">
+        <v>5167</v>
+      </c>
+    </row>
+    <row r="5161" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A5161" s="1" t="s">
+        <v>5168</v>
+      </c>
+    </row>
+    <row r="5162" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A5162" s="1" t="s">
+        <v>5169</v>
+      </c>
+    </row>
+    <row r="5163" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A5163" s="1" t="s">
+        <v>5170</v>
+      </c>
+    </row>
+    <row r="5164" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A5164" s="1" t="s">
+        <v>5171</v>
+      </c>
+    </row>
+    <row r="5165" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A5165" s="1" t="s">
+        <v>5172</v>
+      </c>
+    </row>
+    <row r="5166" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A5166" s="1" t="s">
+        <v>5173</v>
+      </c>
+    </row>
+    <row r="5167" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A5167" s="1" t="s">
+        <v>5174</v>
+      </c>
+    </row>
+    <row r="5168" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A5168" s="1" t="s">
+        <v>5175</v>
+      </c>
+    </row>
+    <row r="5169" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A5169" s="1" t="s">
+        <v>5176</v>
+      </c>
+    </row>
+    <row r="5170" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A5170" s="1" t="s">
+        <v>5177</v>
+      </c>
+    </row>
+    <row r="5171" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A5171" s="1" t="s">
+        <v>5178</v>
+      </c>
+    </row>
+    <row r="5172" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A5172" s="1" t="s">
+        <v>5179</v>
+      </c>
+    </row>
+    <row r="5173" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A5173" s="1" t="s">
+        <v>5180</v>
+      </c>
+    </row>
+    <row r="5174" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A5174" s="1" t="s">
+        <v>5181</v>
+      </c>
+    </row>
+    <row r="5175" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A5175" s="1" t="s">
+        <v>5182</v>
+      </c>
+    </row>
+    <row r="5176" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A5176" s="1" t="s">
+        <v>5183</v>
+      </c>
+    </row>
+    <row r="5177" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A5177" s="1" t="s">
+        <v>5184</v>
+      </c>
+    </row>
+    <row r="5178" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A5178" s="1" t="s">
+        <v>5185</v>
+      </c>
+    </row>
+    <row r="5179" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A5179" s="1" t="s">
+        <v>5186</v>
+      </c>
+    </row>
+    <row r="5180" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A5180" s="1" t="s">
+        <v>5187</v>
+      </c>
+    </row>
+    <row r="5181" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A5181" s="1" t="s">
+        <v>5188</v>
+      </c>
+    </row>
+    <row r="5182" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A5182" s="1" t="s">
+        <v>5189</v>
+      </c>
+    </row>
+    <row r="5183" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A5183" s="1" t="s">
+        <v>5190</v>
+      </c>
+    </row>
+    <row r="5184" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A5184" s="1" t="s">
+        <v>5191</v>
+      </c>
+    </row>
+    <row r="5185" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A5185" s="1" t="s">
+        <v>5192</v>
+      </c>
+    </row>
+    <row r="5186" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A5186" s="1" t="s">
+        <v>5193</v>
+      </c>
+    </row>
+    <row r="5187" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A5187" s="1" t="s">
+        <v>5194</v>
+      </c>
+    </row>
+    <row r="5188" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A5188" s="1" t="s">
+        <v>5195</v>
+      </c>
+    </row>
+    <row r="5189" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A5189" s="1" t="s">
+        <v>5196</v>
+      </c>
+    </row>
+    <row r="5190" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A5190" s="1" t="s">
+        <v>5197</v>
+      </c>
+    </row>
+    <row r="5191" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A5191" s="1" t="s">
+        <v>5198</v>
+      </c>
+    </row>
+    <row r="5192" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A5192" s="1" t="s">
+        <v>5199</v>
+      </c>
+    </row>
+    <row r="5193" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A5193" s="1" t="s">
+        <v>5200</v>
+      </c>
+    </row>
+    <row r="5194" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A5194" s="1" t="s">
+        <v>5201</v>
+      </c>
+    </row>
+    <row r="5195" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A5195" s="1" t="s">
+        <v>5202</v>
+      </c>
+    </row>
+    <row r="5196" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A5196" s="1" t="s">
+        <v>5203</v>
+      </c>
+    </row>
+    <row r="5197" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A5197" s="1" t="s">
+        <v>5204</v>
+      </c>
+    </row>
+    <row r="5198" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A5198" s="1" t="s">
+        <v>5205</v>
+      </c>
+    </row>
+    <row r="5199" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A5199" s="1" t="s">
+        <v>5206</v>
+      </c>
+    </row>
+    <row r="5200" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A5200" s="1" t="s">
+        <v>5207</v>
+      </c>
+    </row>
+    <row r="5201" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A5201" s="1" t="s">
+        <v>5208</v>
+      </c>
+    </row>
+    <row r="5202" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A5202" s="1" t="s">
+        <v>5209</v>
+      </c>
+    </row>
+    <row r="5203" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A5203" s="1" t="s">
+        <v>5210</v>
+      </c>
+    </row>
+    <row r="5204" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A5204" s="1" t="s">
+        <v>5211</v>
+      </c>
+    </row>
+    <row r="5205" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A5205" s="1" t="s">
+        <v>5212</v>
+      </c>
+    </row>
+    <row r="5206" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A5206" s="1" t="s">
+        <v>5213</v>
+      </c>
+    </row>
+    <row r="5207" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A5207" s="1" t="s">
+        <v>5214</v>
+      </c>
+    </row>
+    <row r="5208" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A5208" s="1" t="s">
+        <v>5215</v>
+      </c>
+    </row>
+    <row r="5209" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A5209" s="1" t="s">
+        <v>5216</v>
+      </c>
+    </row>
+    <row r="5210" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A5210" s="1" t="s">
+        <v>5217</v>
+      </c>
+    </row>
+    <row r="5211" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A5211" s="1" t="s">
+        <v>5218</v>
+      </c>
+    </row>
+    <row r="5212" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A5212" s="1" t="s">
+        <v>5219</v>
+      </c>
+    </row>
+    <row r="5213" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A5213" s="1" t="s">
+        <v>5220</v>
+      </c>
+    </row>
+    <row r="5214" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A5214" s="1" t="s">
+        <v>5221</v>
+      </c>
+    </row>
+    <row r="5215" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A5215" s="1" t="s">
+        <v>5222</v>
+      </c>
+    </row>
+    <row r="5216" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A5216" s="1" t="s">
+        <v>5223</v>
       </c>
     </row>
   </sheetData>

</xml_diff>